<commit_message>
PLSstatic werkt, maar heb aanpassingen aan factor_model en pls_model gedaan waardoor PCAstatic en PCAcombined niet meer werken. Nu eerst PLSstatic results, dan PLScombined, dan oude versie terughalen voor PCAstatic en PCAcombined.
</commit_message>
<xml_diff>
--- a/PLSstatic_predicted_factors_matrix_10.xlsx
+++ b/PLSstatic_predicted_factors_matrix_10.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:AV11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,6 +449,135 @@
       <c r="E1" s="1" t="n">
         <v>4</v>
       </c>
+      <c r="F1" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="AG1" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="AH1" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="AI1" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="AJ1" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="AK1" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="AL1" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="AM1" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="AN1" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="AO1" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="AP1" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="AQ1" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="AR1" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="AS1" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="AT1" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="AU1" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="AV1" s="1" t="n">
+        <v>47</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -466,6 +595,135 @@
       <c r="E2" t="n">
         <v>-0.8126726569083593</v>
       </c>
+      <c r="F2" t="n">
+        <v>-0.7127058846178177</v>
+      </c>
+      <c r="G2" t="n">
+        <v>-0.6368593498677785</v>
+      </c>
+      <c r="H2" t="n">
+        <v>-0.5826594989757308</v>
+      </c>
+      <c r="I2" t="n">
+        <v>-0.5475342432629735</v>
+      </c>
+      <c r="J2" t="n">
+        <v>-0.5287874314322437</v>
+      </c>
+      <c r="K2" t="n">
+        <v>-0.5242802760925858</v>
+      </c>
+      <c r="L2" t="n">
+        <v>-0.5316719774378847</v>
+      </c>
+      <c r="M2" t="n">
+        <v>-0.5492362271935772</v>
+      </c>
+      <c r="N2" t="n">
+        <v>-0.5747787695140458</v>
+      </c>
+      <c r="O2" t="n">
+        <v>-0.6066812779467359</v>
+      </c>
+      <c r="P2" t="n">
+        <v>-0.6435085631424426</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>-0.6839984287537385</v>
+      </c>
+      <c r="R2" t="n">
+        <v>-0.7270493630351472</v>
+      </c>
+      <c r="S2" t="n">
+        <v>-0.7717085516873493</v>
+      </c>
+      <c r="T2" t="n">
+        <v>-0.817159000310558</v>
+      </c>
+      <c r="U2" t="n">
+        <v>-0.8627072907364255</v>
+      </c>
+      <c r="V2" t="n">
+        <v>-0.9077718275634237</v>
+      </c>
+      <c r="W2" t="n">
+        <v>-0.9518716970110721</v>
+      </c>
+      <c r="X2" t="n">
+        <v>-0.9946161894047464</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>-1.035694985863938</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>-1.074869118478518</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>-1.111962267248245</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>-1.146853145250794</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>-1.179468230037367</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>-1.209775100147021</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>-1.237776333746826</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>-1.263503941777046</v>
+      </c>
+      <c r="AG2" t="n">
+        <v>-1.287014310163962</v>
+      </c>
+      <c r="AH2" t="n">
+        <v>-1.308383662419297</v>
+      </c>
+      <c r="AI2" t="n">
+        <v>-1.326776851948833</v>
+      </c>
+      <c r="AJ2" t="n">
+        <v>-1.343244488447969</v>
+      </c>
+      <c r="AK2" t="n">
+        <v>-1.358839106140091</v>
+      </c>
+      <c r="AL2" t="n">
+        <v>-1.372711891296535</v>
+      </c>
+      <c r="AM2" t="n">
+        <v>-1.384987314849786</v>
+      </c>
+      <c r="AN2" t="n">
+        <v>-1.395790465966665</v>
+      </c>
+      <c r="AO2" t="n">
+        <v>-1.405245328591579</v>
+      </c>
+      <c r="AP2" t="n">
+        <v>-1.413473336046605</v>
+      </c>
+      <c r="AQ2" t="n">
+        <v>-1.420592018751119</v>
+      </c>
+      <c r="AR2" t="n">
+        <v>-1.427610080801911</v>
+      </c>
+      <c r="AS2" t="n">
+        <v>-1.43278280868182</v>
+      </c>
+      <c r="AT2" t="n">
+        <v>-1.437177479143633</v>
+      </c>
+      <c r="AU2" t="n">
+        <v>-1.440886262481569</v>
+      </c>
+      <c r="AV2" t="n">
+        <v>-1.443994836371908</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -483,6 +741,135 @@
       <c r="E3" t="n">
         <v>-1.000677193359527</v>
       </c>
+      <c r="F3" t="n">
+        <v>-1.094037453233063</v>
+      </c>
+      <c r="G3" t="n">
+        <v>-1.162439452490761</v>
+      </c>
+      <c r="H3" t="n">
+        <v>-1.206369783497253</v>
+      </c>
+      <c r="I3" t="n">
+        <v>-1.227554795131039</v>
+      </c>
+      <c r="J3" t="n">
+        <v>-1.226101928948145</v>
+      </c>
+      <c r="K3" t="n">
+        <v>-1.207102119423047</v>
+      </c>
+      <c r="L3" t="n">
+        <v>-1.173603518270857</v>
+      </c>
+      <c r="M3" t="n">
+        <v>-1.13038265212921</v>
+      </c>
+      <c r="N3" t="n">
+        <v>-1.077997668869004</v>
+      </c>
+      <c r="O3" t="n">
+        <v>-1.018824216896874</v>
+      </c>
+      <c r="P3" t="n">
+        <v>-0.9550001835384455</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>-0.8884130737314827</v>
+      </c>
+      <c r="R3" t="n">
+        <v>-0.8207001500407483</v>
+      </c>
+      <c r="S3" t="n">
+        <v>-0.7532556719412015</v>
+      </c>
+      <c r="T3" t="n">
+        <v>-0.6872443500388845</v>
+      </c>
+      <c r="U3" t="n">
+        <v>-0.6236178417009587</v>
+      </c>
+      <c r="V3" t="n">
+        <v>-0.5631329223313276</v>
+      </c>
+      <c r="W3" t="n">
+        <v>-0.5063704335629802</v>
+      </c>
+      <c r="X3" t="n">
+        <v>-0.4537543153081561</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>-0.4055702450226489</v>
+      </c>
+      <c r="Z3" t="n">
+        <v>-0.3619833131279023</v>
+      </c>
+      <c r="AA3" t="n">
+        <v>-0.3230554469237625</v>
+      </c>
+      <c r="AB3" t="n">
+        <v>-0.2887610155236722</v>
+      </c>
+      <c r="AC3" t="n">
+        <v>-0.2590013633937854</v>
+      </c>
+      <c r="AD3" t="n">
+        <v>-0.2336182256939873</v>
+      </c>
+      <c r="AE3" t="n">
+        <v>-0.2124058939316563</v>
+      </c>
+      <c r="AF3" t="n">
+        <v>-0.1951221406163212</v>
+      </c>
+      <c r="AG3" t="n">
+        <v>-0.1814979369672134</v>
+      </c>
+      <c r="AH3" t="n">
+        <v>-0.1712459903694728</v>
+      </c>
+      <c r="AI3" t="n">
+        <v>-0.1638720843110506</v>
+      </c>
+      <c r="AJ3" t="n">
+        <v>-0.1593259922624866</v>
+      </c>
+      <c r="AK3" t="n">
+        <v>-0.1574904795557916</v>
+      </c>
+      <c r="AL3" t="n">
+        <v>-0.1578137257680642</v>
+      </c>
+      <c r="AM3" t="n">
+        <v>-0.1600124073862595</v>
+      </c>
+      <c r="AN3" t="n">
+        <v>-0.1638141595297882</v>
+      </c>
+      <c r="AO3" t="n">
+        <v>-0.1689610021381414</v>
+      </c>
+      <c r="AP3" t="n">
+        <v>-0.1752111355584708</v>
+      </c>
+      <c r="AQ3" t="n">
+        <v>-0.1823406784546625</v>
+      </c>
+      <c r="AR3" t="n">
+        <v>-0.1904371496461199</v>
+      </c>
+      <c r="AS3" t="n">
+        <v>-0.1987332483187436</v>
+      </c>
+      <c r="AT3" t="n">
+        <v>-0.2073419259503489</v>
+      </c>
+      <c r="AU3" t="n">
+        <v>-0.2161155366077292</v>
+      </c>
+      <c r="AV3" t="n">
+        <v>-0.2249247569154702</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -500,6 +887,135 @@
       <c r="E4" t="n">
         <v>0.4523383873478526</v>
       </c>
+      <c r="F4" t="n">
+        <v>0.3409082708156608</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.2419968660213504</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.1548893095943221</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.07892302906355927</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.01340403759649484</v>
+      </c>
+      <c r="K4" t="n">
+        <v>-0.04207402682694401</v>
+      </c>
+      <c r="L4" t="n">
+        <v>-0.08834367817022329</v>
+      </c>
+      <c r="M4" t="n">
+        <v>-0.1265621809616565</v>
+      </c>
+      <c r="N4" t="n">
+        <v>-0.1573785532713981</v>
+      </c>
+      <c r="O4" t="n">
+        <v>-0.1815378666106389</v>
+      </c>
+      <c r="P4" t="n">
+        <v>-0.1997641695351689</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>-0.2127500357325555</v>
+      </c>
+      <c r="R4" t="n">
+        <v>-0.221151931150511</v>
+      </c>
+      <c r="S4" t="n">
+        <v>-0.2255829982353136</v>
+      </c>
+      <c r="T4" t="n">
+        <v>-0.2266148507601621</v>
+      </c>
+      <c r="U4" t="n">
+        <v>-0.2247755755064177</v>
+      </c>
+      <c r="V4" t="n">
+        <v>-0.2205497148794558</v>
+      </c>
+      <c r="W4" t="n">
+        <v>-0.2143789011801999</v>
+      </c>
+      <c r="X4" t="n">
+        <v>-0.2066629029963182</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>-0.1977609693122791</v>
+      </c>
+      <c r="Z4" t="n">
+        <v>-0.187992163233534</v>
+      </c>
+      <c r="AA4" t="n">
+        <v>-0.1776410886060252</v>
+      </c>
+      <c r="AB4" t="n">
+        <v>-0.1669555175372416</v>
+      </c>
+      <c r="AC4" t="n">
+        <v>-0.1561498616066077</v>
+      </c>
+      <c r="AD4" t="n">
+        <v>-0.1454073618488516</v>
+      </c>
+      <c r="AE4" t="n">
+        <v>-0.1348822669452688</v>
+      </c>
+      <c r="AF4" t="n">
+        <v>-0.1247020564945878</v>
+      </c>
+      <c r="AG4" t="n">
+        <v>-0.1149696873444307</v>
+      </c>
+      <c r="AH4" t="n">
+        <v>-0.1057658333670654</v>
+      </c>
+      <c r="AI4" t="n">
+        <v>-0.09683178650575582</v>
+      </c>
+      <c r="AJ4" t="n">
+        <v>-0.0885783922918601</v>
+      </c>
+      <c r="AK4" t="n">
+        <v>-0.08130328086594361</v>
+      </c>
+      <c r="AL4" t="n">
+        <v>-0.07470792797994971</v>
+      </c>
+      <c r="AM4" t="n">
+        <v>-0.06878363603611017</v>
+      </c>
+      <c r="AN4" t="n">
+        <v>-0.06352051371204265</v>
+      </c>
+      <c r="AO4" t="n">
+        <v>-0.058900831788689</v>
+      </c>
+      <c r="AP4" t="n">
+        <v>-0.05490014559280217</v>
+      </c>
+      <c r="AQ4" t="n">
+        <v>-0.0514882311866264</v>
+      </c>
+      <c r="AR4" t="n">
+        <v>-0.04877461538420853</v>
+      </c>
+      <c r="AS4" t="n">
+        <v>-0.04644134234884283</v>
+      </c>
+      <c r="AT4" t="n">
+        <v>-0.04457873024798897</v>
+      </c>
+      <c r="AU4" t="n">
+        <v>-0.04315009904186414</v>
+      </c>
+      <c r="AV4" t="n">
+        <v>-0.0421153151440406</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -517,6 +1033,135 @@
       <c r="E5" t="n">
         <v>0.4686903319544485</v>
       </c>
+      <c r="F5" t="n">
+        <v>0.3822598525022731</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.2982216233382413</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.218879409198593</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.1456564661463725</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.0791494866595905</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.02037691108001792</v>
+      </c>
+      <c r="L5" t="n">
+        <v>-0.03074311583773536</v>
+      </c>
+      <c r="M5" t="n">
+        <v>-0.07471632669499197</v>
+      </c>
+      <c r="N5" t="n">
+        <v>-0.1119283339932841</v>
+      </c>
+      <c r="O5" t="n">
+        <v>-0.1427697206880918</v>
+      </c>
+      <c r="P5" t="n">
+        <v>-0.1676946021914541</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>-0.1871943579833259</v>
+      </c>
+      <c r="R5" t="n">
+        <v>-0.2017775974324105</v>
+      </c>
+      <c r="S5" t="n">
+        <v>-0.2119561864520516</v>
+      </c>
+      <c r="T5" t="n">
+        <v>-0.2182330301650928</v>
+      </c>
+      <c r="U5" t="n">
+        <v>-0.2210945856209508</v>
+      </c>
+      <c r="V5" t="n">
+        <v>-0.2210051159569925</v>
+      </c>
+      <c r="W5" t="n">
+        <v>-0.2184026245130288</v>
+      </c>
+      <c r="X5" t="n">
+        <v>-0.2136961109164524</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>-0.2072638736604278</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>-0.1994529384372932</v>
+      </c>
+      <c r="AA5" t="n">
+        <v>-0.1905775747329109</v>
+      </c>
+      <c r="AB5" t="n">
+        <v>-0.1809211139608374</v>
+      </c>
+      <c r="AC5" t="n">
+        <v>-0.170736033743198</v>
+      </c>
+      <c r="AD5" t="n">
+        <v>-0.1602449634906206</v>
+      </c>
+      <c r="AE5" t="n">
+        <v>-0.1496419881740833</v>
+      </c>
+      <c r="AF5" t="n">
+        <v>-0.1390941555553777</v>
+      </c>
+      <c r="AG5" t="n">
+        <v>-0.1287431335649033</v>
+      </c>
+      <c r="AH5" t="n">
+        <v>-0.118706943638327</v>
+      </c>
+      <c r="AI5" t="n">
+        <v>-0.1087332703953082</v>
+      </c>
+      <c r="AJ5" t="n">
+        <v>-0.09931801756412759</v>
+      </c>
+      <c r="AK5" t="n">
+        <v>-0.0908005150054509</v>
+      </c>
+      <c r="AL5" t="n">
+        <v>-0.08285867110441923</v>
+      </c>
+      <c r="AM5" t="n">
+        <v>-0.07552599705023558</v>
+      </c>
+      <c r="AN5" t="n">
+        <v>-0.0688188518401651</v>
+      </c>
+      <c r="AO5" t="n">
+        <v>-0.06274185953743938</v>
+      </c>
+      <c r="AP5" t="n">
+        <v>-0.05728978832656743</v>
+      </c>
+      <c r="AQ5" t="n">
+        <v>-0.05244933465452259</v>
+      </c>
+      <c r="AR5" t="n">
+        <v>-0.04835957320544237</v>
+      </c>
+      <c r="AS5" t="n">
+        <v>-0.04466600187185724</v>
+      </c>
+      <c r="AT5" t="n">
+        <v>-0.04151123524104382</v>
+      </c>
+      <c r="AU5" t="n">
+        <v>-0.03886018035440754</v>
+      </c>
+      <c r="AV5" t="n">
+        <v>-0.03667696235687739</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -534,6 +1179,135 @@
       <c r="E6" t="n">
         <v>-0.3908770708943669</v>
       </c>
+      <c r="F6" t="n">
+        <v>-0.3116555002812539</v>
+      </c>
+      <c r="G6" t="n">
+        <v>-0.246248663979397</v>
+      </c>
+      <c r="H6" t="n">
+        <v>-0.1928336301189485</v>
+      </c>
+      <c r="I6" t="n">
+        <v>-0.1495587148794167</v>
+      </c>
+      <c r="J6" t="n">
+        <v>-0.1138645837582322</v>
+      </c>
+      <c r="K6" t="n">
+        <v>-0.08538692465814253</v>
+      </c>
+      <c r="L6" t="n">
+        <v>-0.06274786656743407</v>
+      </c>
+      <c r="M6" t="n">
+        <v>-0.04526426729268342</v>
+      </c>
+      <c r="N6" t="n">
+        <v>-0.03146920168545941</v>
+      </c>
+      <c r="O6" t="n">
+        <v>-0.02064606718240385</v>
+      </c>
+      <c r="P6" t="n">
+        <v>-0.01221099477750989</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>-0.005689693833538191</v>
+      </c>
+      <c r="R6" t="n">
+        <v>-0.0006981689822552033</v>
+      </c>
+      <c r="S6" t="n">
+        <v>0.003074393620911267</v>
+      </c>
+      <c r="T6" t="n">
+        <v>0.005878934733095144</v>
+      </c>
+      <c r="U6" t="n">
+        <v>0.007918188319026201</v>
+      </c>
+      <c r="V6" t="n">
+        <v>0.009355934306564541</v>
+      </c>
+      <c r="W6" t="n">
+        <v>0.01032447163830026</v>
+      </c>
+      <c r="X6" t="n">
+        <v>0.01093063820548114</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>0.01126063375777636</v>
+      </c>
+      <c r="Z6" t="n">
+        <v>0.0113839260492585</v>
+      </c>
+      <c r="AA6" t="n">
+        <v>0.01135617960548698</v>
+      </c>
+      <c r="AB6" t="n">
+        <v>0.01122223172961628</v>
+      </c>
+      <c r="AC6" t="n">
+        <v>0.01101776080239828</v>
+      </c>
+      <c r="AD6" t="n">
+        <v>0.01077092697152017</v>
+      </c>
+      <c r="AE6" t="n">
+        <v>0.01050371915095496</v>
+      </c>
+      <c r="AF6" t="n">
+        <v>0.01023305395338173</v>
+      </c>
+      <c r="AG6" t="n">
+        <v>0.009971677938609327</v>
+      </c>
+      <c r="AH6" t="n">
+        <v>0.009728947738366939</v>
+      </c>
+      <c r="AI6" t="n">
+        <v>0.009476465941157898</v>
+      </c>
+      <c r="AJ6" t="n">
+        <v>0.009243717825045022</v>
+      </c>
+      <c r="AK6" t="n">
+        <v>0.009076467260774398</v>
+      </c>
+      <c r="AL6" t="n">
+        <v>0.008947699441757764</v>
+      </c>
+      <c r="AM6" t="n">
+        <v>0.008857181297561285</v>
+      </c>
+      <c r="AN6" t="n">
+        <v>0.008801910726221534</v>
+      </c>
+      <c r="AO6" t="n">
+        <v>0.008778536127569335</v>
+      </c>
+      <c r="AP6" t="n">
+        <v>0.008783559428717627</v>
+      </c>
+      <c r="AQ6" t="n">
+        <v>0.008813563880614203</v>
+      </c>
+      <c r="AR6" t="n">
+        <v>0.008918359073950347</v>
+      </c>
+      <c r="AS6" t="n">
+        <v>0.008993768276831092</v>
+      </c>
+      <c r="AT6" t="n">
+        <v>0.00908119396140547</v>
+      </c>
+      <c r="AU6" t="n">
+        <v>0.009177814721348505</v>
+      </c>
+      <c r="AV6" t="n">
+        <v>0.009281629602016058</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -551,6 +1325,135 @@
       <c r="E7" t="n">
         <v>0.1248686829731715</v>
       </c>
+      <c r="F7" t="n">
+        <v>0.1443941743803165</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.1541920199325688</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.1563702135977237</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.1528266394321618</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0.1436685067559563</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.1320782353988648</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0.1190998524869072</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0.1066204542580405</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0.09374819450448496</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0.08094270481476366</v>
+      </c>
+      <c r="P7" t="n">
+        <v>0.06853644686490055</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>0.05676125404792186</v>
+      </c>
+      <c r="R7" t="n">
+        <v>0.04577075006971294</v>
+      </c>
+      <c r="S7" t="n">
+        <v>0.03565772194761823</v>
+      </c>
+      <c r="T7" t="n">
+        <v>0.02646889597295651</v>
+      </c>
+      <c r="U7" t="n">
+        <v>0.01821652630273822</v>
+      </c>
+      <c r="V7" t="n">
+        <v>0.01088746711763929</v>
+      </c>
+      <c r="W7" t="n">
+        <v>0.004450268453456627</v>
+      </c>
+      <c r="X7" t="n">
+        <v>-0.001139308550309637</v>
+      </c>
+      <c r="Y7" t="n">
+        <v>-0.005934025689901228</v>
+      </c>
+      <c r="Z7" t="n">
+        <v>-0.009992119149098165</v>
+      </c>
+      <c r="AA7" t="n">
+        <v>-0.01337429916478801</v>
+      </c>
+      <c r="AB7" t="n">
+        <v>-0.01614213909492729</v>
+      </c>
+      <c r="AC7" t="n">
+        <v>-0.01835673332746637</v>
+      </c>
+      <c r="AD7" t="n">
+        <v>-0.02007763383885164</v>
+      </c>
+      <c r="AE7" t="n">
+        <v>-0.02136207568517516</v>
+      </c>
+      <c r="AF7" t="n">
+        <v>-0.02226442980003182</v>
+      </c>
+      <c r="AG7" t="n">
+        <v>-0.02283583154536394</v>
+      </c>
+      <c r="AH7" t="n">
+        <v>-0.0231239612266706</v>
+      </c>
+      <c r="AI7" t="n">
+        <v>-0.02295011744489571</v>
+      </c>
+      <c r="AJ7" t="n">
+        <v>-0.02262103034761644</v>
+      </c>
+      <c r="AK7" t="n">
+        <v>-0.02238082543939588</v>
+      </c>
+      <c r="AL7" t="n">
+        <v>-0.02199519963854679</v>
+      </c>
+      <c r="AM7" t="n">
+        <v>-0.0214973912737093</v>
+      </c>
+      <c r="AN7" t="n">
+        <v>-0.02091708394838066</v>
+      </c>
+      <c r="AO7" t="n">
+        <v>-0.02028008887103526</v>
+      </c>
+      <c r="AP7" t="n">
+        <v>-0.01960861802321228</v>
+      </c>
+      <c r="AQ7" t="n">
+        <v>-0.01892159871687736</v>
+      </c>
+      <c r="AR7" t="n">
+        <v>-0.01839970501647662</v>
+      </c>
+      <c r="AS7" t="n">
+        <v>-0.01769479243345304</v>
+      </c>
+      <c r="AT7" t="n">
+        <v>-0.01702174945534336</v>
+      </c>
+      <c r="AU7" t="n">
+        <v>-0.01638778689056138</v>
+      </c>
+      <c r="AV7" t="n">
+        <v>-0.01579822332450969</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -568,6 +1471,135 @@
       <c r="E8" t="n">
         <v>0.3466183140066855</v>
       </c>
+      <c r="F8" t="n">
+        <v>0.2750469192576975</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.2185251832439718</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.1744367345406729</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.1404822544672064</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0.113716555785882</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.09384611548293743</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0.07929707360667361</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0.0693439826665383</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0.0622113097958162</v>
+      </c>
+      <c r="O8" t="n">
+        <v>0.05716669315940294</v>
+      </c>
+      <c r="P8" t="n">
+        <v>0.05362814887189653</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>0.051139598193353</v>
+      </c>
+      <c r="R8" t="n">
+        <v>0.04934949611333497</v>
+      </c>
+      <c r="S8" t="n">
+        <v>0.04799182401904355</v>
+      </c>
+      <c r="T8" t="n">
+        <v>0.04686996080202829</v>
+      </c>
+      <c r="U8" t="n">
+        <v>0.04584294783567462</v>
+      </c>
+      <c r="V8" t="n">
+        <v>0.04481395600800407</v>
+      </c>
+      <c r="W8" t="n">
+        <v>0.04372066430720562</v>
+      </c>
+      <c r="X8" t="n">
+        <v>0.04252729390058851</v>
+      </c>
+      <c r="Y8" t="n">
+        <v>0.04121807617304026</v>
+      </c>
+      <c r="Z8" t="n">
+        <v>0.03979195211644518</v>
+      </c>
+      <c r="AA8" t="n">
+        <v>0.03825816167412631</v>
+      </c>
+      <c r="AB8" t="n">
+        <v>0.03663288890685281</v>
+      </c>
+      <c r="AC8" t="n">
+        <v>0.03493658725177148</v>
+      </c>
+      <c r="AD8" t="n">
+        <v>0.03319188917268312</v>
+      </c>
+      <c r="AE8" t="n">
+        <v>0.03142202039963538</v>
+      </c>
+      <c r="AF8" t="n">
+        <v>0.02964962889418644</v>
+      </c>
+      <c r="AG8" t="n">
+        <v>0.02789595046856673</v>
+      </c>
+      <c r="AH8" t="n">
+        <v>0.02618021660751199</v>
+      </c>
+      <c r="AI8" t="n">
+        <v>0.02432064133234373</v>
+      </c>
+      <c r="AJ8" t="n">
+        <v>0.02258201885914114</v>
+      </c>
+      <c r="AK8" t="n">
+        <v>0.02113636197437171</v>
+      </c>
+      <c r="AL8" t="n">
+        <v>0.01976977908149747</v>
+      </c>
+      <c r="AM8" t="n">
+        <v>0.01849108513363152</v>
+      </c>
+      <c r="AN8" t="n">
+        <v>0.01730670715806237</v>
+      </c>
+      <c r="AO8" t="n">
+        <v>0.01623850881779175</v>
+      </c>
+      <c r="AP8" t="n">
+        <v>0.01525464630155796</v>
+      </c>
+      <c r="AQ8" t="n">
+        <v>0.01437101730386935</v>
+      </c>
+      <c r="AR8" t="n">
+        <v>0.01368346007994758</v>
+      </c>
+      <c r="AS8" t="n">
+        <v>0.01297330607744069</v>
+      </c>
+      <c r="AT8" t="n">
+        <v>0.01236028906447747</v>
+      </c>
+      <c r="AU8" t="n">
+        <v>0.01183899993465769</v>
+      </c>
+      <c r="AV8" t="n">
+        <v>0.011403425409099</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -585,6 +1617,135 @@
       <c r="E9" t="n">
         <v>0.2558881634735482</v>
       </c>
+      <c r="F9" t="n">
+        <v>0.2116557432969029</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.1679119123338894</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.1265282740860376</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.08869582480822127</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0.05452414304209986</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.02536189690224464</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0.001100404096775283</v>
+      </c>
+      <c r="M9" t="n">
+        <v>-0.01860863835490427</v>
+      </c>
+      <c r="N9" t="n">
+        <v>-0.03426365341578811</v>
+      </c>
+      <c r="O9" t="n">
+        <v>-0.04619909271619289</v>
+      </c>
+      <c r="P9" t="n">
+        <v>-0.05479363001733207</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>-0.06044398352803033</v>
+      </c>
+      <c r="R9" t="n">
+        <v>-0.06354654968442457</v>
+      </c>
+      <c r="S9" t="n">
+        <v>-0.06448420621285132</v>
+      </c>
+      <c r="T9" t="n">
+        <v>-0.06361791315624349</v>
+      </c>
+      <c r="U9" t="n">
+        <v>-0.06128153099508024</v>
+      </c>
+      <c r="V9" t="n">
+        <v>-0.05777892359736819</v>
+      </c>
+      <c r="W9" t="n">
+        <v>-0.05338276065061465</v>
+      </c>
+      <c r="X9" t="n">
+        <v>-0.04833453163936252</v>
+      </c>
+      <c r="Y9" t="n">
+        <v>-0.04284540976461659</v>
+      </c>
+      <c r="Z9" t="n">
+        <v>-0.03709755125239969</v>
+      </c>
+      <c r="AA9" t="n">
+        <v>-0.03124613502775545</v>
+      </c>
+      <c r="AB9" t="n">
+        <v>-0.02542134082275557</v>
+      </c>
+      <c r="AC9" t="n">
+        <v>-0.01973039813293731</v>
+      </c>
+      <c r="AD9" t="n">
+        <v>-0.01425975671208657</v>
+      </c>
+      <c r="AE9" t="n">
+        <v>-0.009077237898921512</v>
+      </c>
+      <c r="AF9" t="n">
+        <v>-0.004234121396335588</v>
+      </c>
+      <c r="AG9" t="n">
+        <v>0.0002328606440901489</v>
+      </c>
+      <c r="AH9" t="n">
+        <v>0.004299654867096507</v>
+      </c>
+      <c r="AI9" t="n">
+        <v>0.007918808772079303</v>
+      </c>
+      <c r="AJ9" t="n">
+        <v>0.0111067795690136</v>
+      </c>
+      <c r="AK9" t="n">
+        <v>0.01395891678255176</v>
+      </c>
+      <c r="AL9" t="n">
+        <v>0.01640166046883935</v>
+      </c>
+      <c r="AM9" t="n">
+        <v>0.01845077923691283</v>
+      </c>
+      <c r="AN9" t="n">
+        <v>0.02012675541052491</v>
+      </c>
+      <c r="AO9" t="n">
+        <v>0.02144096932323513</v>
+      </c>
+      <c r="AP9" t="n">
+        <v>0.02244367316540739</v>
+      </c>
+      <c r="AQ9" t="n">
+        <v>0.02314978560709546</v>
+      </c>
+      <c r="AR9" t="n">
+        <v>0.02375024272161576</v>
+      </c>
+      <c r="AS9" t="n">
+        <v>0.02390691774450989</v>
+      </c>
+      <c r="AT9" t="n">
+        <v>0.02385686562344016</v>
+      </c>
+      <c r="AU9" t="n">
+        <v>0.02362666455089663</v>
+      </c>
+      <c r="AV9" t="n">
+        <v>0.02324158458294278</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -602,6 +1763,135 @@
       <c r="E10" t="n">
         <v>0.1041894243199889</v>
       </c>
+      <c r="F10" t="n">
+        <v>0.1097191819058061</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.1035176773062652</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.09031753363549232</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.07343996138450548</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0.05418988457539471</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0.03554277451409114</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0.01837656977223994</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0.003429465785517592</v>
+      </c>
+      <c r="N10" t="n">
+        <v>-0.009585794548363761</v>
+      </c>
+      <c r="O10" t="n">
+        <v>-0.02055119439828005</v>
+      </c>
+      <c r="P10" t="n">
+        <v>-0.02947895056039055</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>-0.03646656665796356</v>
+      </c>
+      <c r="R10" t="n">
+        <v>-0.04166422203875488</v>
+      </c>
+      <c r="S10" t="n">
+        <v>-0.04525165539670845</v>
+      </c>
+      <c r="T10" t="n">
+        <v>-0.04742157040903826</v>
+      </c>
+      <c r="U10" t="n">
+        <v>-0.04836839385913687</v>
+      </c>
+      <c r="V10" t="n">
+        <v>-0.04828069883940597</v>
+      </c>
+      <c r="W10" t="n">
+        <v>-0.04733632618535637</v>
+      </c>
+      <c r="X10" t="n">
+        <v>-0.04569944880762531</v>
+      </c>
+      <c r="Y10" t="n">
+        <v>-0.04351901723882556</v>
+      </c>
+      <c r="Z10" t="n">
+        <v>-0.04092822676571309</v>
+      </c>
+      <c r="AA10" t="n">
+        <v>-0.03804439080634212</v>
+      </c>
+      <c r="AB10" t="n">
+        <v>-0.03496970047244756</v>
+      </c>
+      <c r="AC10" t="n">
+        <v>-0.03179195267859913</v>
+      </c>
+      <c r="AD10" t="n">
+        <v>-0.02858552248112759</v>
+      </c>
+      <c r="AE10" t="n">
+        <v>-0.02541243682858777</v>
+      </c>
+      <c r="AF10" t="n">
+        <v>-0.02232348864891548</v>
+      </c>
+      <c r="AG10" t="n">
+        <v>-0.01935935168771733</v>
+      </c>
+      <c r="AH10" t="n">
+        <v>-0.01655166838220636</v>
+      </c>
+      <c r="AI10" t="n">
+        <v>-0.01372109321353955</v>
+      </c>
+      <c r="AJ10" t="n">
+        <v>-0.01117028014693566</v>
+      </c>
+      <c r="AK10" t="n">
+        <v>-0.009021532034349938</v>
+      </c>
+      <c r="AL10" t="n">
+        <v>-0.007065917982470971</v>
+      </c>
+      <c r="AM10" t="n">
+        <v>-0.005310409295174899</v>
+      </c>
+      <c r="AN10" t="n">
+        <v>-0.003756241443913668</v>
+      </c>
+      <c r="AO10" t="n">
+        <v>-0.00240027042692184</v>
+      </c>
+      <c r="AP10" t="n">
+        <v>-0.001236506949647939</v>
+      </c>
+      <c r="AQ10" t="n">
+        <v>-0.0002560793716787761</v>
+      </c>
+      <c r="AR10" t="n">
+        <v>0.000547954399290407</v>
+      </c>
+      <c r="AS10" t="n">
+        <v>0.001191791338252147</v>
+      </c>
+      <c r="AT10" t="n">
+        <v>0.001687127183734234</v>
+      </c>
+      <c r="AU10" t="n">
+        <v>0.002047845423638412</v>
+      </c>
+      <c r="AV10" t="n">
+        <v>0.002287644631344234</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -618,6 +1908,135 @@
       </c>
       <c r="E11" t="n">
         <v>-0.01726714791921361</v>
+      </c>
+      <c r="F11" t="n">
+        <v>-0.02199765887798776</v>
+      </c>
+      <c r="G11" t="n">
+        <v>-0.01994462148695538</v>
+      </c>
+      <c r="H11" t="n">
+        <v>-0.01522480631733887</v>
+      </c>
+      <c r="I11" t="n">
+        <v>-0.009966170349517918</v>
+      </c>
+      <c r="J11" t="n">
+        <v>-0.004952835674125144</v>
+      </c>
+      <c r="K11" t="n">
+        <v>-0.001047707891334886</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0.001774519706599377</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0.003697902653720804</v>
+      </c>
+      <c r="N11" t="n">
+        <v>0.004874564177150102</v>
+      </c>
+      <c r="O11" t="n">
+        <v>0.005443681096251077</v>
+      </c>
+      <c r="P11" t="n">
+        <v>0.005543471947685855</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>0.005292982650723817</v>
+      </c>
+      <c r="R11" t="n">
+        <v>0.004806238402178625</v>
+      </c>
+      <c r="S11" t="n">
+        <v>0.004169237013860357</v>
+      </c>
+      <c r="T11" t="n">
+        <v>0.00345075268696566</v>
+      </c>
+      <c r="U11" t="n">
+        <v>0.002703984614153278</v>
+      </c>
+      <c r="V11" t="n">
+        <v>0.001968852359625183</v>
+      </c>
+      <c r="W11" t="n">
+        <v>0.001274254029263214</v>
+      </c>
+      <c r="X11" t="n">
+        <v>0.0006401246930487934</v>
+      </c>
+      <c r="Y11" t="n">
+        <v>8.477736867655767e-05</v>
+      </c>
+      <c r="Z11" t="n">
+        <v>-0.0003928677546293339</v>
+      </c>
+      <c r="AA11" t="n">
+        <v>-0.0007888537437240902</v>
+      </c>
+      <c r="AB11" t="n">
+        <v>-0.001103084665973203</v>
+      </c>
+      <c r="AC11" t="n">
+        <v>-0.001338158836462685</v>
+      </c>
+      <c r="AD11" t="n">
+        <v>-0.001498568055760129</v>
+      </c>
+      <c r="AE11" t="n">
+        <v>-0.001590081167984576</v>
+      </c>
+      <c r="AF11" t="n">
+        <v>-0.001619266023567597</v>
+      </c>
+      <c r="AG11" t="n">
+        <v>-0.001593119831525635</v>
+      </c>
+      <c r="AH11" t="n">
+        <v>-0.001514960149725383</v>
+      </c>
+      <c r="AI11" t="n">
+        <v>-0.001357014351889204</v>
+      </c>
+      <c r="AJ11" t="n">
+        <v>-0.001177589979919729</v>
+      </c>
+      <c r="AK11" t="n">
+        <v>-0.001012842394268752</v>
+      </c>
+      <c r="AL11" t="n">
+        <v>-0.0008247408335172177</v>
+      </c>
+      <c r="AM11" t="n">
+        <v>-0.0006189029145948813</v>
+      </c>
+      <c r="AN11" t="n">
+        <v>-0.000400314511483984</v>
+      </c>
+      <c r="AO11" t="n">
+        <v>-0.00017364362253454</v>
+      </c>
+      <c r="AP11" t="n">
+        <v>5.684558770479263e-05</v>
+      </c>
+      <c r="AQ11" t="n">
+        <v>0.0002874287076968672</v>
+      </c>
+      <c r="AR11" t="n">
+        <v>0.0005224438741196012</v>
+      </c>
+      <c r="AS11" t="n">
+        <v>0.0007417697887237558</v>
+      </c>
+      <c r="AT11" t="n">
+        <v>0.0009549289804457362</v>
+      </c>
+      <c r="AU11" t="n">
+        <v>0.001159107518663397</v>
+      </c>
+      <c r="AV11" t="n">
+        <v>0.001352308701194958</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
out of sample PLS static gefixt, nu PLScombined
</commit_message>
<xml_diff>
--- a/PLSstatic_predicted_factors_matrix_10.xlsx
+++ b/PLSstatic_predicted_factors_matrix_10.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AV11"/>
+  <dimension ref="A1:AU11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -575,9 +575,6 @@
       <c r="AU1" s="1" t="n">
         <v>46</v>
       </c>
-      <c r="AV1" s="1" t="n">
-        <v>47</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -721,9 +718,6 @@
       <c r="AU2" t="n">
         <v>-1.440886262481569</v>
       </c>
-      <c r="AV2" t="n">
-        <v>-1.443994836371908</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -867,9 +861,6 @@
       <c r="AU3" t="n">
         <v>-0.2161155366077292</v>
       </c>
-      <c r="AV3" t="n">
-        <v>-0.2249247569154702</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -1013,9 +1004,6 @@
       <c r="AU4" t="n">
         <v>-0.04315009904186414</v>
       </c>
-      <c r="AV4" t="n">
-        <v>-0.0421153151440406</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -1159,9 +1147,6 @@
       <c r="AU5" t="n">
         <v>-0.03886018035440754</v>
       </c>
-      <c r="AV5" t="n">
-        <v>-0.03667696235687739</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -1305,9 +1290,6 @@
       <c r="AU6" t="n">
         <v>0.009177814721348505</v>
       </c>
-      <c r="AV6" t="n">
-        <v>0.009281629602016058</v>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -1451,9 +1433,6 @@
       <c r="AU7" t="n">
         <v>-0.01638778689056138</v>
       </c>
-      <c r="AV7" t="n">
-        <v>-0.01579822332450969</v>
-      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -1597,9 +1576,6 @@
       <c r="AU8" t="n">
         <v>0.01183899993465769</v>
       </c>
-      <c r="AV8" t="n">
-        <v>0.011403425409099</v>
-      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -1743,9 +1719,6 @@
       <c r="AU9" t="n">
         <v>0.02362666455089663</v>
       </c>
-      <c r="AV9" t="n">
-        <v>0.02324158458294278</v>
-      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -1889,9 +1862,6 @@
       <c r="AU10" t="n">
         <v>0.002047845423638412</v>
       </c>
-      <c r="AV10" t="n">
-        <v>0.002287644631344234</v>
-      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -2034,9 +2004,6 @@
       </c>
       <c r="AU11" t="n">
         <v>0.001159107518663397</v>
-      </c>
-      <c r="AV11" t="n">
-        <v>0.001352308701194958</v>
       </c>
     </row>
   </sheetData>

</xml_diff>